<commit_message>
Adicionado (logF_BusinessProcessName) aos nomes dos arquivos de output.
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Stephano\Documents\UiPath\GAVB\Dealbook\Capture Companies\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0781CD16-5E46-4B0E-B48D-44488A01F515}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{076E476A-8501-48D9-A165-1A70A505BD63}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -216,9 +216,6 @@
     <t>TXT</t>
   </si>
   <si>
-    <t>Capture Companies</t>
-  </si>
-  <si>
     <t>/companies</t>
   </si>
   <si>
@@ -238,6 +235,9 @@
   </si>
   <si>
     <t>Company,Description,Website,Linkedin,Status,Markets,Locations,Investors,Deals,Investments,Investor,Investor URL</t>
+  </si>
+  <si>
+    <t>dealbook_companies</t>
   </si>
 </sst>
 </file>
@@ -605,7 +605,7 @@
   <dimension ref="A1:Z998"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -656,7 +656,7 @@
         <v>43</v>
       </c>
       <c r="B3" t="s">
-        <v>64</v>
+        <v>71</v>
       </c>
       <c r="C3" t="s">
         <v>44</v>
@@ -690,7 +690,7 @@
         <v>60</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C7" s="2"/>
     </row>
@@ -699,7 +699,7 @@
         <v>56</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -707,15 +707,15 @@
         <v>62</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -753,10 +753,10 @@
     </row>
     <row r="17" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B17" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>